<commit_message>
feat: Add Excel preview and enhanced inspection image features
- Add Excel preview functionality for supervisors to view reports before downloading
- Implement image capture and export for First Aid kit inspections
- Enhance ExcelViewer component with flexible display options (zoom, header controls)
- Add new inspector submissions page for form management
- Simplify photo capture workflow to kit-level only in First Aid inspections
- Allow deletion of inspections regardless of status (with ownership restrictions)
- Improve error handling and logging for image export in Fire Extinguisher reports

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/templates/fire-extinguisher-template.xlsx
+++ b/public/templates/fire-extinguisher-template.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aimi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239A802C-6172-404F-B34D-F7B6190CE477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C107193A-A649-4FE2-90FC-BF621454DFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="September - 2025" sheetId="8" r:id="rId1"/>
+    <sheet name="Fire Extinguisher Checklist" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'September - 2025'!$A$1:$S$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Fire Extinguisher Checklist'!$A$1:$S$40</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -471,6 +471,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -515,9 +518,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,8 +893,8 @@
   </sheetPr>
   <dimension ref="A4:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,139 +913,139 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
     </row>
     <row r="8" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="15"/>
     </row>
     <row r="9" spans="1:16" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="18" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="18" t="s">
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="P9" s="20"/>
+      <c r="P9" s="21"/>
     </row>
     <row r="10" spans="1:16" ht="58.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="23" t="s">
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="P10" s="22"/>
+      <c r="P10" s="23"/>
     </row>
     <row r="11" spans="1:16" ht="61.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="24" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="13" t="s">
         <v>42</v>
       </c>
       <c r="J12" s="11" t="s">
@@ -1071,9 +1071,9 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="97.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -1768,15 +1768,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="N12:N13"/>
     <mergeCell ref="A7:P7"/>
@@ -1793,6 +1784,15 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="O12:O13"/>
     <mergeCell ref="P12:P13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="48" orientation="portrait" r:id="rId1"/>
@@ -1801,6 +1801,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="6cc334ba-fc18-470a-9544-3c919287b1c4" xsi:nil="true"/>
@@ -1809,15 +1818,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2070,20 +2070,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5945AF2E-0DBF-4A50-AFFE-E6EE8F247054}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE6D7E7E-BFA6-48DF-9306-FEB98B07A42B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="6cc334ba-fc18-470a-9544-3c919287b1c4"/>
     <ds:schemaRef ds:uri="0290ab27-6b47-46ba-abe3-9fde3578c93d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5945AF2E-0DBF-4A50-AFFE-E6EE8F247054}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>